<commit_message>
Static pivot tables - (blank) row and column #230
</commit_message>
<xml_diff>
--- a/tests/Gauges/Subranges_Multiple.xlsx
+++ b/tests/Gauges/Subranges_Multiple.xlsx
@@ -16,10 +16,10 @@
     <x:sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Customers">'Sheet 1'!$A$4:$I$813</x:definedName>
-    <x:definedName name="Customers_tpl">'Sheet 1'!$A$4:$I$813</x:definedName>
-    <x:definedName name="Customers_Orders_tpl">'Sheet 1'!$A$6:$I$7</x:definedName>
-    <x:definedName name="Customers_Visitors_tpl">'Sheet 1'!$A$10:$I$11</x:definedName>
+    <x:definedName name="Customers_tpl" localSheetId="0">'Sheet 1'!$A$4:$I$812</x:definedName>
+    <x:definedName name="Customers_Orders_tpl" localSheetId="0">'Sheet 1'!$A$6:$I$7</x:definedName>
+    <x:definedName name="Customers_Visitors_tpl" localSheetId="0">'Sheet 1'!$A$10:$I$11</x:definedName>
+    <x:definedName name="Customers">'Sheet 1'!$A$4:$I$812</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="191029"/>
   <x:extLst>
@@ -10525,11 +10525,8 @@
         <x:f>Subtotal(9,D807:D810)</x:f>
       </x:c>
     </x:row>
-    <x:row r="813" spans="1:9">
-      <x:c r="E813" s="2" t="s"/>
-    </x:row>
-    <x:row r="815" spans="1:9">
-      <x:c r="I815" s="3" t="s"/>
+    <x:row r="814" spans="1:9">
+      <x:c r="I814" s="3" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="499">

</xml_diff>

<commit_message>
Static pivot tables - (blank) row and column #230 (#232)
</commit_message>
<xml_diff>
--- a/tests/Gauges/Subranges_Multiple.xlsx
+++ b/tests/Gauges/Subranges_Multiple.xlsx
@@ -16,10 +16,10 @@
     <x:sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames>
-    <x:definedName name="Customers">'Sheet 1'!$A$4:$I$813</x:definedName>
-    <x:definedName name="Customers_tpl">'Sheet 1'!$A$4:$I$813</x:definedName>
-    <x:definedName name="Customers_Orders_tpl">'Sheet 1'!$A$6:$I$7</x:definedName>
-    <x:definedName name="Customers_Visitors_tpl">'Sheet 1'!$A$10:$I$11</x:definedName>
+    <x:definedName name="Customers_tpl" localSheetId="0">'Sheet 1'!$A$4:$I$812</x:definedName>
+    <x:definedName name="Customers_Orders_tpl" localSheetId="0">'Sheet 1'!$A$6:$I$7</x:definedName>
+    <x:definedName name="Customers_Visitors_tpl" localSheetId="0">'Sheet 1'!$A$10:$I$11</x:definedName>
+    <x:definedName name="Customers">'Sheet 1'!$A$4:$I$812</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="191029"/>
   <x:extLst>
@@ -10525,11 +10525,8 @@
         <x:f>Subtotal(9,D807:D810)</x:f>
       </x:c>
     </x:row>
-    <x:row r="813" spans="1:9">
-      <x:c r="E813" s="2" t="s"/>
-    </x:row>
-    <x:row r="815" spans="1:9">
-      <x:c r="I815" s="3" t="s"/>
+    <x:row r="814" spans="1:9">
+      <x:c r="I814" s="3" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="499">

</xml_diff>